<commit_message>
Training with a Softmax
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.ginn\PycharmProjects\StemDetector\StemDetector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.ginn\PycharmProjects\StemDetector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C8DC7AC-EC2C-46E8-8414-CCD2C96A540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D64933-52B8-4A74-9EE2-E9CD8019F429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{DAB9BE0A-60A2-4994-87A3-C8748D7E3373}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{DAB9BE0A-60A2-4994-87A3-C8748D7E3373}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Mask RCNN Acc:</t>
+    <t>Recall</t>
   </si>
   <si>
-    <t>Encoder-Decoder F1:</t>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Mask RCNN Accuracy</t>
+  </si>
+  <si>
+    <t>Encoder-Decoder F1 score</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mask RCNN Acc:</c:v>
+                  <c:v>Mask RCNN Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -225,7 +231,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Encoder-Decoder F1:</c:v>
+                  <c:v>Encoder-Decoder F1 score</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -300,6 +306,139 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B9DD-40BA-A672-CF488D449914}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Encoder-Decoder Recall</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.96319999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93769999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88680000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83150000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-040D-4839-A824-2A56AAEDC7C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Encoder-Decoder Precision</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.99299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98809999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96020000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-040D-4839-A824-2A56AAEDC7C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -430,6 +569,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1035,15 +1205,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1368,15 +1538,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF561009-3D62-4446-AC2A-2085D3AB7571}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1402,7 +1572,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>0.80878821270000001</v>
@@ -1425,7 +1595,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>0.97789999999999999</v>
@@ -1444,6 +1614,52 @@
       </c>
       <c r="G3" s="1">
         <v>0.88680000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.96319999999999995</v>
+      </c>
+      <c r="C4">
+        <v>0.95789999999999997</v>
+      </c>
+      <c r="D4">
+        <v>0.93769999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.91379999999999995</v>
+      </c>
+      <c r="F4">
+        <v>0.88680000000000003</v>
+      </c>
+      <c r="G4">
+        <v>0.83150000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.98809999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.98470000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.98089999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.96020000000000005</v>
+      </c>
+      <c r="G5">
+        <v>0.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working well with mAP calculation
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.ginn\PycharmProjects\StemDetector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D64933-52B8-4A74-9EE2-E9CD8019F429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F8DAE8-4ED4-4C81-B327-26152420F459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{DAB9BE0A-60A2-4994-87A3-C8748D7E3373}"/>
   </bookViews>
@@ -42,17 +42,17 @@
     <t>Precision</t>
   </si>
   <si>
-    <t>Mask RCNN Accuracy</t>
+    <t>Mask RCNN mAP</t>
   </si>
   <si>
-    <t>Encoder-Decoder F1 score</t>
+    <t>Encoder-Decoder mAP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,16 +66,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,11 +112,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -97,6 +141,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -129,6 +185,78 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mask RCNN vs Growing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Point mAP</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -136,30 +264,264 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Encoder-Decoder mAP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="sq">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="47625" cap="sq">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:gradFill rotWithShape="1">
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="accent2">
+                        <a:satMod val="103000"/>
+                        <a:lumMod val="102000"/>
+                        <a:tint val="94000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="50000">
+                      <a:schemeClr val="accent2">
+                        <a:satMod val="110000"/>
+                        <a:lumMod val="100000"/>
+                        <a:shade val="100000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="99000"/>
+                        <a:satMod val="120000"/>
+                        <a:shade val="78000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+                <a:ln w="47625">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="63000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9470-4A21-BADD-26751C688725}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.98470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9788</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95679999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91169999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B9DD-40BA-A672-CF488D449914}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mask RCNN Accuracy</c:v>
+                  <c:v>Mask RCNN mAP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="47625">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -222,226 +584,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Encoder-Decoder F1 score</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$G$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.97789999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.9728</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.96060000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.94620000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.92200000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.88680000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B9DD-40BA-A672-CF488D449914}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Encoder-Decoder Recall</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$G$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.96319999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95789999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.93769999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.91379999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.88680000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.83150000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-040D-4839-A824-2A56AAEDC7C9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Encoder-Decoder Precision</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$5:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.99299999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98809999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.98470000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.98089999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.96020000000000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.95</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-040D-4839-A824-2A56AAEDC7C9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -450,6 +592,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="352467256"/>
         <c:axId val="352470536"/>
@@ -461,6 +604,64 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Max</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Occlusion Percentage</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -469,9 +670,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -485,9 +686,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -509,6 +709,8 @@
         <c:axId val="352470536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -516,9 +718,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -526,6 +728,64 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>mean</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Average Precision (MAP)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -544,9 +804,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -570,7 +829,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -586,9 +845,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -612,17 +870,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -685,35 +954,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -721,26 +988,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -749,9 +1024,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -770,14 +1044,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -786,45 +1052,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -836,31 +1092,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -878,21 +1132,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -902,20 +1153,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -929,14 +1180,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -950,9 +1201,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -966,12 +1216,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -983,9 +1227,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1000,108 +1244,115 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1113,12 +1364,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1134,7 +1392,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1143,9 +1400,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1155,7 +1411,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1163,9 +1419,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1176,9 +1432,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1190,12 +1445,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1210,8 +1459,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
@@ -1538,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF561009-3D62-4446-AC2A-2085D3AB7571}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,70 +1846,69 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.97789999999999999</v>
+      <c r="B3" s="4">
+        <v>0.98470000000000002</v>
       </c>
       <c r="C3" s="1">
-        <v>0.9728</v>
+        <v>0.9788</v>
       </c>
       <c r="D3" s="1">
-        <v>0.96060000000000001</v>
+        <v>0.95679999999999998</v>
       </c>
       <c r="E3" s="1">
-        <v>0.94620000000000004</v>
+        <v>0.95369999999999999</v>
       </c>
       <c r="F3" s="1">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.88680000000000003</v>
-      </c>
+        <v>0.91169999999999995</v>
+      </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>0.96319999999999995</v>
-      </c>
-      <c r="C4">
-        <v>0.95789999999999997</v>
-      </c>
-      <c r="D4">
-        <v>0.93769999999999998</v>
-      </c>
-      <c r="E4">
-        <v>0.91379999999999995</v>
-      </c>
-      <c r="F4">
-        <v>0.88680000000000003</v>
-      </c>
-      <c r="G4">
-        <v>0.83150000000000002</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="C5">
-        <v>0.98809999999999998</v>
-      </c>
-      <c r="D5">
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>0.8115</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.67269999999999996</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.63649999999999995</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.57589999999999997</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.52149999999999996</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.48970000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>0.98470000000000002</v>
       </c>
-      <c r="E5">
-        <v>0.98089999999999999</v>
-      </c>
-      <c r="F5">
-        <v>0.96020000000000005</v>
-      </c>
-      <c r="G5">
-        <v>0.95</v>
-      </c>
+      <c r="B10" s="5">
+        <v>0.9788</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.95679999999999998</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5">
+        <v>0.91169999999999995</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>